<commit_message>
updated excel and testng
</commit_message>
<xml_diff>
--- a/testData/timetracker_glenn_v2.xlsx
+++ b/testData/timetracker_glenn_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="53">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product</t>
   </si>
   <si>
     <t xml:space="preserve">TC001_TimeTracker_Login_ValidCredentials</t>
@@ -340,10 +343,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -362,54 +365,57 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -541,27 +547,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="8" t="n">
         <v>45071</v>
@@ -573,18 +579,18 @@
         <v>0.708333333333333</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="8" t="n">
         <v>45071</v>
@@ -596,18 +602,18 @@
         <v>0.708333333333333</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="8" t="n">
         <v>45071</v>
@@ -619,18 +625,18 @@
         <v>0.708333333333333</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="8" t="n">
         <v>45071</v>
@@ -642,18 +648,18 @@
         <v>0.708333333333333</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>45071</v>
@@ -665,18 +671,18 @@
         <v>0.708333333333333</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="8" t="n">
         <v>45071</v>
@@ -688,18 +694,18 @@
         <v>0.708333333333333</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="8" t="n">
         <v>45071</v>
@@ -711,7 +717,7 @@
         <v>0.708333333333333</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -754,51 +760,51 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -819,7 +825,7 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -840,473 +846,473 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>